<commit_message>
Update Combat Narrative Guide.xlsx
</commit_message>
<xml_diff>
--- a/Combat Narrative Guide.xlsx
+++ b/Combat Narrative Guide.xlsx
@@ -8,30 +8,42 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Foundry VTT\Data\modules\combat-narration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33BBC622-2424-4196-BBB5-38BFC6777328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5DD70D6-D656-4D76-939F-4BF34B56047C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25017" yWindow="-118" windowWidth="25370" windowHeight="13667" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25017" yWindow="-118" windowWidth="25370" windowHeight="13667" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OnDamageRoll" sheetId="1" r:id="rId1"/>
     <sheet name="Not Effective Expansion" sheetId="5" r:id="rId2"/>
     <sheet name="Monster Specific Expansion" sheetId="4" r:id="rId3"/>
+    <sheet name="Fear Expansion" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Monster Specific Expansion'!$A$1:$B$141</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">OnDamageRoll!$A$1:$B$316</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="1304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1346" uniqueCount="1344">
   <si>
     <t>Filename</t>
   </si>
@@ -3943,6 +3955,126 @@
   </si>
   <si>
     <t>Your weapon whooshes past their torso. A tremor runs through their body.</t>
+  </si>
+  <si>
+    <t>fear_success_001.oog</t>
+  </si>
+  <si>
+    <t>The terror claws at their mind, but they force it back with a ragged breath.</t>
+  </si>
+  <si>
+    <t>fear_success_002.oog</t>
+  </si>
+  <si>
+    <t>fear_success_003.oog</t>
+  </si>
+  <si>
+    <t>Cold dread flashes through them, quickly smothered by sheer will.</t>
+  </si>
+  <si>
+    <t>fear_success_004.oog</t>
+  </si>
+  <si>
+    <t>Their heart races, but they refuse to give fear ground.</t>
+  </si>
+  <si>
+    <t>fear_success_005.oog</t>
+  </si>
+  <si>
+    <t>The horror presses in, only to be beaten back by grim resolve.</t>
+  </si>
+  <si>
+    <t>fear_success_006.oog</t>
+  </si>
+  <si>
+    <t>A flicker of panic dies as they lock their gaze forward.</t>
+  </si>
+  <si>
+    <t>fear_success_007.oog</t>
+  </si>
+  <si>
+    <t>Sweat beads as they steel themselves against the creeping terror.</t>
+  </si>
+  <si>
+    <t>fear_success_008.oog</t>
+  </si>
+  <si>
+    <t>The fear whispers promises of death, but they do not listen.</t>
+  </si>
+  <si>
+    <t>fear_success_009.oog</t>
+  </si>
+  <si>
+    <t>fear_success_010.oog</t>
+  </si>
+  <si>
+    <t>fear_fail_001.oog</t>
+  </si>
+  <si>
+    <t>fear_fail_002.oog</t>
+  </si>
+  <si>
+    <t>fear_fail_003.oog</t>
+  </si>
+  <si>
+    <t>fear_fail_004.oog</t>
+  </si>
+  <si>
+    <t>fear_fail_005.oog</t>
+  </si>
+  <si>
+    <t>fear_fail_006.oog</t>
+  </si>
+  <si>
+    <t>fear_fail_007.oog</t>
+  </si>
+  <si>
+    <t>fear_fail_008.oog</t>
+  </si>
+  <si>
+    <t>fear_fail_009.oog</t>
+  </si>
+  <si>
+    <t>fear_fail_010.oog</t>
+  </si>
+  <si>
+    <t>Their form shakes, but they steady themselves before panic takes hold.</t>
+  </si>
+  <si>
+    <t>They refuse to be controlled by fear.</t>
+  </si>
+  <si>
+    <t>Horrifying thoughts pick at their mind, but they are rejected on false premise.</t>
+  </si>
+  <si>
+    <t>Terror floods their mind, drowning all reason!</t>
+  </si>
+  <si>
+    <t>Their eyes widen as panic takes full control!</t>
+  </si>
+  <si>
+    <t>A strangled gasp escapes as the fear locks in!</t>
+  </si>
+  <si>
+    <t>The horror overwhelms them, shaking them to their core!</t>
+  </si>
+  <si>
+    <t>Their courage shatters, leaving only raw panic behind!</t>
+  </si>
+  <si>
+    <t>They recoil in terror, instincts screaming to flee!</t>
+  </si>
+  <si>
+    <t>Their breath comes in short, frantic bursts as fear consumes them!</t>
+  </si>
+  <si>
+    <t>Their mind begins to spiral into a living nightmare!</t>
+  </si>
+  <si>
+    <t>Fear crushes their resolve, leaving them trembling and exposed!</t>
+  </si>
+  <si>
+    <t>Panic takes root in their mind, heart hammering wildly!</t>
   </si>
 </sst>
 </file>
@@ -4289,8 +4421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E436"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -9578,4 +9710,224 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B38C8AD-3C55-4D25-998B-F386DA8AF4EA}">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34.33203125" customWidth="1"/>
+    <col min="2" max="2" width="112" customWidth="1"/>
+    <col min="3" max="3" width="87" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="26.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="24.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>1306</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1331</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>1307</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>1311</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="23.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>1313</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="20.3" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="23.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>1319</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>1333</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>1321</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>1334</v>
+      </c>
+      <c r="C11" t="str">
+        <f>_xlfn.CONCAT("&lt;emotion value='excited'/&gt;",B11,)</f>
+        <v>&lt;emotion value='excited'/&gt;Terror floods their mind, drowning all reason!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>1322</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>1335</v>
+      </c>
+      <c r="C12" t="str">
+        <f>_xlfn.CONCAT("&lt;emotion value='excited'/&gt;",B12,)</f>
+        <v>&lt;emotion value='excited'/&gt;Their eyes widen as panic takes full control!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>1323</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>1336</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" ref="C13:C19" si="0">_xlfn.CONCAT("&lt;emotion value='excited'/&gt;",B13,)</f>
+        <v>&lt;emotion value='excited'/&gt;A strangled gasp escapes as the fear locks in!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>1324</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>1337</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;emotion value='excited'/&gt;The horror overwhelms them, shaking them to their core!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>1325</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>1338</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;emotion value='excited'/&gt;Their courage shatters, leaving only raw panic behind!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>1326</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>1339</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;emotion value='excited'/&gt;They recoil in terror, instincts screaming to flee!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>1327</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;emotion value='excited'/&gt;Their breath comes in short, frantic bursts as fear consumes them!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>1328</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>1341</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;emotion value='excited'/&gt;Their mind begins to spiral into a living nightmare!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>1329</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>1343</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;emotion value='excited'/&gt;Panic takes root in their mind, heart hammering wildly!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>1342</v>
+      </c>
+      <c r="C20" t="str">
+        <f>_xlfn.CONCAT("&lt;emotion value='excited'/&gt;",B20,)</f>
+        <v>&lt;emotion value='excited'/&gt;Fear crushes their resolve, leaving them trembling and exposed!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>